<commit_message>
Finalizando para uma isoterma
</commit_message>
<xml_diff>
--- a/Dados/Nova pasta/K2CO3_dados_entrada_303.xlsx
+++ b/Dados/Nova pasta/K2CO3_dados_entrada_303.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LABSIMULAÇÃO\Meu Drive\Papers\Manuscript Modeling solubility with Jafo\New electrolytes_DataBase\Dados entrada isoT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\Desktop\Salt_Solubility_MS\Dados\Nova pasta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73964138-F80A-4963-874C-9F2EC1C7B119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A34588-A59E-488E-B98A-A70F267235D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4515" yWindow="1290" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parametros" sheetId="1" r:id="rId1"/>
@@ -721,7 +721,7 @@
   <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D10"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -750,7 +750,7 @@
     </row>
     <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="11">
-        <v>303.14999999999998</v>
+        <v>313.14999999999998</v>
       </c>
       <c r="B2" s="15">
         <v>1</v>

</xml_diff>